<commit_message>
Initial integration of label gateway
</commit_message>
<xml_diff>
--- a/workingdir/label_data.xlsx
+++ b/workingdir/label_data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="ModelTable" sheetId="1" state="visible" r:id="rId2"/>
@@ -15,7 +15,8 @@
     <sheet name="ItemTable" sheetId="5" state="visible" r:id="rId6"/>
     <sheet name="UnitTable" sheetId="6" state="visible" r:id="rId7"/>
     <sheet name="YearTable" sheetId="7" state="visible" r:id="rId8"/>
-    <sheet name="ValueSwapTable" sheetId="8" state="visible" r:id="rId9"/>
+    <sheet name="RegionFixTable" sheetId="8" state="visible" r:id="rId9"/>
+    <sheet name="ValueFixTable" sheetId="9" state="visible" r:id="rId10"/>
   </sheets>
   <definedNames>
     <definedName function="false" hidden="true" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">ScenarioTable!$A$1:$C$56</definedName>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1154" uniqueCount="481">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1166" uniqueCount="487">
   <si>
     <t xml:space="preserve">No</t>
   </si>
@@ -1473,6 +1474,24 @@
   </si>
   <si>
     <t xml:space="preserve">Year</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fix</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#div/0!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">n/a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">na</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nan</t>
   </si>
 </sst>
 </file>
@@ -1796,7 +1815,7 @@
   </sheetPr>
   <dimension ref="A1:D62"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D47" activeCellId="0" sqref="D47"/>
     </sheetView>
   </sheetViews>
@@ -7020,7 +7039,58 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.3671875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="19.25"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>122</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Arial,Regular"&amp;10&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Arial,Regular"&amp;10Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:C35"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
@@ -7028,7 +7098,211 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.3671875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>482</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>483</v>
+      </c>
+      <c r="C2" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>484</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>485</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>486</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="n">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="n">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="n">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="n">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="n">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="n">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="n">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="n">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="n">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="n">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="n">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="n">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="n">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="n">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="n">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="0" t="n">
+        <v>34</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>

</xml_diff>